<commit_message>
Add 9 more test case for BOA Homepage
</commit_message>
<xml_diff>
--- a/com.bankofamerica/src/test/resources/BankOfAmerica.xlsx
+++ b/com.bankofamerica/src/test/resources/BankOfAmerica.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafiz\IDEA Project\Team1BootCamp\base\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdaziz/IdeaProjects/Team1BootCamp/com.bankofamerica/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4722EE68-90EB-42C0-AF92-D8B589C2F532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF6B3D5-5E44-0C41-9144-511A83A2062B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
-    <sheet name="Expedia" sheetId="1" r:id="rId1"/>
-    <sheet name="Ebay" sheetId="2" r:id="rId2"/>
-    <sheet name="CBSSports" sheetId="3" r:id="rId3"/>
+    <sheet name="BOALogin" sheetId="1" r:id="rId1"/>
+    <sheet name="PasswordReset" sheetId="2" r:id="rId2"/>
+    <sheet name="URL" sheetId="3" r:id="rId3"/>
     <sheet name="ATT" sheetId="4" r:id="rId4"/>
     <sheet name="BankOfAmerica" sheetId="5" r:id="rId5"/>
     <sheet name="BMWUSA" sheetId="6" r:id="rId6"/>
@@ -47,19 +47,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>userid123</t>
+  </si>
+  <si>
+    <t>password123</t>
+  </si>
+  <si>
+    <t>accoun</t>
+  </si>
+  <si>
+    <t>ssn</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://locators.bankofamerica.com/</t>
+  </si>
+  <si>
+    <t>https://www.bankofamerica.com/</t>
+  </si>
+  <si>
+    <t>TestData</t>
+  </si>
+  <si>
+    <t>12603</t>
+  </si>
+  <si>
+    <t>https://locators.bankofamerica.com/?q=12603</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -82,13 +135,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -401,12 +458,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F16D271-5906-41EE-853E-85EA245B6942}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -419,7 +499,7 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -433,7 +513,7 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -447,7 +527,7 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -461,7 +541,7 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -475,7 +555,7 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -483,28 +563,104 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9751B09C-FE73-4F13-A91B-81E55B55AAEA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A517B4-AB0A-4E50-8324-F3955FA294DA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="54" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{A17EDC32-25C9-5A43-9F39-B0ACD156F38B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -517,7 +673,7 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -531,9 +687,9 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +707,7 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -563,7 +719,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -575,7 +731,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -587,7 +743,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add 2 more test case for BOA Homepage
</commit_message>
<xml_diff>
--- a/com.bankofamerica/src/test/resources/BankOfAmerica.xlsx
+++ b/com.bankofamerica/src/test/resources/BankOfAmerica.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdaziz/IdeaProjects/Team1BootCamp/com.bankofamerica/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF6B3D5-5E44-0C41-9144-511A83A2062B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E543DC6-C9DB-7B41-99AE-E96A1193C61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="BOALogin" sheetId="1" r:id="rId1"/>
     <sheet name="PasswordReset" sheetId="2" r:id="rId2"/>
     <sheet name="URL" sheetId="3" r:id="rId3"/>
-    <sheet name="ATT" sheetId="4" r:id="rId4"/>
+    <sheet name="FilterOptions" sheetId="4" r:id="rId4"/>
     <sheet name="BankOfAmerica" sheetId="5" r:id="rId5"/>
     <sheet name="BMWUSA" sheetId="6" r:id="rId6"/>
     <sheet name="Trulia" sheetId="7" r:id="rId7"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>A</t>
   </si>
@@ -95,6 +95,81 @@
   </si>
   <si>
     <t>https://locators.bankofamerica.com/?q=12603</t>
+  </si>
+  <si>
+    <t>Optios</t>
+  </si>
+  <si>
+    <t>Drive-thru ATM</t>
+  </si>
+  <si>
+    <t>Walk-up ATM</t>
+  </si>
+  <si>
+    <t>Cardless ATM</t>
+  </si>
+  <si>
+    <t>ATM accepts deposits and credit card payments</t>
+  </si>
+  <si>
+    <t>ATM cash withdrawals only (deposits not accepted)</t>
+  </si>
+  <si>
+    <t>ATM located inside</t>
+  </si>
+  <si>
+    <t>Dedicated Business Teller</t>
+  </si>
+  <si>
+    <t>Glass barrier at Customer Service desk</t>
+  </si>
+  <si>
+    <t>Drive-thru Teller Services</t>
+  </si>
+  <si>
+    <t>Video Conferencing</t>
+  </si>
+  <si>
+    <t>Express financial center</t>
+  </si>
+  <si>
+    <t>Advanced Center™ with Video Chat</t>
+  </si>
+  <si>
+    <t>Accepts appointments</t>
+  </si>
+  <si>
+    <t>Financial Solutions Advisor</t>
+  </si>
+  <si>
+    <t>Home Loans Specialist</t>
+  </si>
+  <si>
+    <t>Centralized Small Business Banker</t>
+  </si>
+  <si>
+    <t>Notary</t>
+  </si>
+  <si>
+    <t>Commercial Deposits Accepted</t>
+  </si>
+  <si>
+    <t>Night Deposit Accepted</t>
+  </si>
+  <si>
+    <t>Change Orders</t>
+  </si>
+  <si>
+    <t>ATM Services Available</t>
+  </si>
+  <si>
+    <t>Open Saturdays</t>
+  </si>
+  <si>
+    <t>Open Sundays</t>
+  </si>
+  <si>
+    <t>Currently open</t>
   </si>
 </sst>
 </file>
@@ -616,7 +691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A517B4-AB0A-4E50-8324-F3955FA294DA}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -667,14 +742,143 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0464987E-CA86-496F-AFAF-2580C40BA720}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <dimension ref="A1:A25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add 5 more test case for BOA Homepage
</commit_message>
<xml_diff>
--- a/com.bankofamerica/src/test/resources/BankOfAmerica.xlsx
+++ b/com.bankofamerica/src/test/resources/BankOfAmerica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdaziz/IdeaProjects/Team1BootCamp/com.bankofamerica/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3599042B-386A-3747-94E2-20180C98DED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680F1CE0-CA17-754F-BFC4-B6E56586EA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="BOALogin" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="FilterOptions" sheetId="4" r:id="rId4"/>
     <sheet name="NavigationBarMenu" sheetId="5" r:id="rId5"/>
     <sheet name="countyList" sheetId="6" r:id="rId6"/>
-    <sheet name="Trulia" sheetId="7" r:id="rId7"/>
+    <sheet name="ManageAppointment" sheetId="7" r:id="rId7"/>
     <sheet name="AirBNB" sheetId="8" r:id="rId8"/>
     <sheet name="OverStock" sheetId="9" r:id="rId9"/>
     <sheet name="ESPN" sheetId="10" r:id="rId10"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>ID</t>
   </si>
@@ -206,6 +206,18 @@
   </si>
   <si>
     <t>CARTER, TN</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>osman@yahoo.com</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>736475372</t>
   </si>
 </sst>
 </file>
@@ -999,7 +1011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5674FF68-7C81-4A9C-99FE-C7E070DBCFFA}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1035,12 +1047,38 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC436034-E141-4F6F-A259-658744C38455}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{0D6A8198-E1A7-4B4A-BE5B-83BA0FEF5B79}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added some test cases BankOfAmerica
</commit_message>
<xml_diff>
--- a/com.bankofamerica/src/test/resources/BankOfAmerica.xlsx
+++ b/com.bankofamerica/src/test/resources/BankOfAmerica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janna\IdeaProjects\Team1BootCamp\com.bankofamerica\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DEF184-35AF-4CA1-9F11-07131CC87A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED1823D-D656-45BA-8124-E07742FADC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="899" firstSheet="7" activeTab="7" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="MobileBankingNavbarElemnts" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="PaymentTransfer" sheetId="5" r:id="rId5"/>
     <sheet name="CardManagement" sheetId="6" r:id="rId6"/>
     <sheet name="BreadCrumb" sheetId="7" r:id="rId7"/>
-    <sheet name="AirBNB" sheetId="8" r:id="rId8"/>
+    <sheet name="TestResult" sheetId="8" r:id="rId8"/>
     <sheet name="OverStock" sheetId="9" r:id="rId9"/>
     <sheet name="ESPN" sheetId="10" r:id="rId10"/>
     <sheet name="Verizon" sheetId="11" r:id="rId11"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>MobileBankingNavbarElemnts</t>
   </si>
@@ -143,6 +143,21 @@
   </si>
   <si>
     <t>Online Banking and Mobile Banking Features</t>
+  </si>
+  <si>
+    <t>testScrollLeft</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>Alerts</t>
+  </si>
+  <si>
+    <t>testScrollRight</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -496,7 +511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F16D271-5906-41EE-853E-85EA245B6942}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -853,17 +868,41 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F06E338-1C0F-45E0-B136-3FC6897D7CEC}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
-    </sheetView>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>